<commit_message>
Updated the program to add the resulting data to excel
</commit_message>
<xml_diff>
--- a/BigCommerceBatchLoad.xlsx
+++ b/BigCommerceBatchLoad.xlsx
@@ -14,21 +14,22 @@
   <sheets>
     <sheet name="From BC to Avalara" sheetId="1" r:id="rId1"/>
     <sheet name="From Avalara to BC" sheetId="2" r:id="rId2"/>
+    <sheet name="avalara_migration-11-9-17-no-tr" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" fullPrecision="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t>merchant_name</t>
   </si>
@@ -163,6 +164,30 @@
   </si>
   <si>
     <t>AvaTax Software License Key</t>
+  </si>
+  <si>
+    <t>AvaTaxSoftwareLicenseKey</t>
+  </si>
+  <si>
+    <t>98101</t>
+  </si>
+  <si>
+    <t>2061112222</t>
+  </si>
+  <si>
+    <t>2000191382</t>
+  </si>
+  <si>
+    <t>D57D0C60AEB80D07</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>2062223333</t>
+  </si>
+  <si>
+    <t>Error Message</t>
   </si>
 </sst>
 </file>
@@ -203,16 +228,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -517,9 +540,11 @@
     <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="24.375" customWidth="1"/>
+    <col min="19" max="19" width="28.25" customWidth="1"/>
+    <col min="20" max="20" width="51.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +602,11 @@
       <c r="S1" t="s">
         <v>44</v>
       </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -597,8 +625,8 @@
       <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="G2">
-        <v>98101</v>
+      <c r="G2" t="s">
+        <v>46</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
@@ -612,8 +640,8 @@
       <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L2">
-        <v>2061112222</v>
+      <c r="L2" t="s">
+        <v>47</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
@@ -627,11 +655,11 @@
       <c r="P2" t="s">
         <v>22</v>
       </c>
-      <c r="Q2">
-        <v>98101</v>
+      <c r="Q2" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -650,8 +678,8 @@
       <c r="F3" t="s">
         <v>42</v>
       </c>
-      <c r="G3">
-        <v>10000</v>
+      <c r="G3" t="s">
+        <v>50</v>
       </c>
       <c r="H3" t="s">
         <v>39</v>
@@ -665,8 +693,8 @@
       <c r="K3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L3">
-        <v>2062223333</v>
+      <c r="L3" t="s">
+        <v>51</v>
       </c>
       <c r="M3" t="s">
         <v>38</v>
@@ -680,8 +708,8 @@
       <c r="P3" t="s">
         <v>22</v>
       </c>
-      <c r="Q3">
-        <v>98101</v>
+      <c r="Q3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -690,6 +718,7 @@
     <hyperlink ref="K3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -772,4 +801,188 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>